<commit_message>
added scraped\_at timestamp to detailed facility records in ZorgkaartDetailsSpider
</commit_message>
<xml_diff>
--- a/ZorgkaartScrapy/data/zorgkaart_details.xlsx
+++ b/ZorgkaartScrapy/data/zorgkaart_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>plaats</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>scraped_at</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -483,33 +488,38 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Medisch Pedicure Landgraaf</t>
+          <t>Hallux Medisch Pedicure</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/medisch-pedicurepraktijk-medisch-pedicure-landgraaf-landgraaf-10070714</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/medisch-pedicurepraktijk-hallux-medisch-pedicure-maastricht-10048434</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Kerkstraat</t>
+          <t>Victor de Steursstraat</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>6374HH</t>
+          <t>6217KP</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Landgraaf</t>
+          <t>Maastricht</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
         </is>
       </c>
     </row>
@@ -521,33 +531,38 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hallux Medisch Pedicure</t>
+          <t>Medisch Pedicure Landgraaf</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/medisch-pedicurepraktijk-hallux-medisch-pedicure-maastricht-10048434</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/medisch-pedicurepraktijk-medisch-pedicure-landgraaf-landgraaf-10070714</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Victor de Steursstraat</t>
+          <t>Kerkstraat</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>25</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>6217KP</t>
+          <t>6374HH</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Maastricht</t>
+          <t>Landgraaf</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
         </is>
       </c>
     </row>
@@ -586,6 +601,11 @@
       <c r="H4" t="inlineStr">
         <is>
           <t>Baarlo</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added new results from spider 3
</commit_message>
<xml_diff>
--- a/ZorgkaartScrapy/data/zorgkaart_details.xlsx
+++ b/ZorgkaartScrapy/data/zorgkaart_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,38 +483,38 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>(Medisch) Pedicurepraktijk</t>
+          <t>Arbo- en reïntegratiebedrijf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hallux Medisch Pedicure</t>
+          <t>Herman Spanjaard, zelfstandig bedrijfsarts</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/medisch-pedicurepraktijk-hallux-medisch-pedicure-maastricht-10048434</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-herman-spanjaard-zelfstandig-bedrijfsarts-halfweg-3063069</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Victor de Steursstraat</t>
+          <t>Schoolstraat</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>6217KP</t>
+          <t>1165HC</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Maastricht</t>
+          <t>Halfweg</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -526,38 +526,38 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>(Medisch) Pedicurepraktijk</t>
+          <t>Arbo- en reïntegratiebedrijf</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Medisch Pedicure Landgraaf</t>
+          <t>Equilar</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/medisch-pedicurepraktijk-medisch-pedicure-landgraaf-landgraaf-10070714</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-equilar-eindhoven-10015888</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Kerkstraat</t>
+          <t>Le Havre</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>6374HH</t>
+          <t>5627ST</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Landgraaf</t>
+          <t>Eindhoven</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -569,41 +569,1660 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>(Medisch) Pedicurepraktijk</t>
+          <t>Arbo- en reïntegratiebedrijf</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>H. Donkersteeg</t>
+          <t>Bötger Bedrijfsarts</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/medisch-pedicurepraktijk-h-donkersteeg-baarlo-10038724</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-botger-bedrijfsarts-heerenveen-3049886</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Kuinderdyk</t>
+          <t>Haskeruitgang</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>109</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>8372VK</t>
+          <t>8447CK</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Baarlo</t>
+          <t>Heerenveen</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Dr. R.V. A-Tjak, Geregistreerd Bedrijfsarts, Westland/Den Haag, tevens Rijbewijskeuringen</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-dr-r-v-a-tjak-geregistreerd-bedrijfsarts-westland-den-haag-tevens-rijbewijskeuringen-naaldwijk-3058085</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Galgepad</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2671MV</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Naaldwijk</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Zorg van de Zaak Den Bosch</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-zorg-van-de-zaak-den-bosch-s-hertogenbosch-100747</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Bruistensingel</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>5232AC</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>'s-Hertogenbosch</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Kalteren Advies</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-kalteren-advies-deventer-3051143</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Rombout Verhulstlaan</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>7425NX</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Deventer</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Hemke.biz</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-hemke-biz-amsterdam-3055781</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Anne Kooistrahof</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1106WG</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Amsterdam</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Marco Straatman, bedrijfsarts</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-marco-straatman-bedrijfsarts-almere-10012969</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Richthuisstraat</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1335XD</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Almere</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Arbo Unie, vestiging Nijmegen</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-arbo-unie-vestiging-nijmegen-nijmegen-101006</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Kerkenbos</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>6546BB</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nijmegen</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Marco Straatman, bedrijfsarts, locatie Hilversum</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-marco-straatman-bedrijfsarts-locatie-hilversum-hilversum-10012970</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Diependaalselaan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>337</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1215KG</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Hilversum</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Natuurlijkbeter Artsenpraktijk</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-natuurlijkbeter-artsenpraktijk-sleeuwijk-219514</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Hoekeinde</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>4254LM</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Sleeuwijk</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Plan B Bedrijfsgezondheidszorg</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-plan-b-bedrijfsgezondheidszorg-zwolle-10016938</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Zuiderkerkstraat</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>8011HG</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Zwolle</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Orthomanuele Geneeskundige Praktijk Leeuwarden</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-orthomanuele-geneeskundige-praktijk-leeuwarden-leeuwarden-3048632</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Wiardaplantage</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>8939AA</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Leeuwarden</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Praktijk Drs A. Qureshi</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-praktijk-drs-a-qureshi-rotterdam-10006208</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Terbregseweg</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>3056JS</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Rotterdam</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Praktijk Pronk voor Musculosketale geneeskunde</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-praktijk-pronk-voor-musculosketale-geneeskunde-sneek-200488</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Harmen Sytstrastraat</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>8602TM</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Sneek</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Senden Medical Services</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-senden-medical-services-sittard-229548</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Linde</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>6131GG</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Sittard</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Ton van Os Bedrijfsarts</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-ton-van-os-bedrijfsarts-uden-3049508</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Artillerieweg</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>5403PB</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Uden</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Rob de Jong, arts orthomanuele geneeskunde</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-rob-de-jong-arts-orthomanuele-geneeskunde-de-wijk-228668</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Dorpsstraat</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>7957AT</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>de Wijk</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Praktijk Brunsting</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-praktijk-brunsting-nijmegen-3031266</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Sloetstraat</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>6524AS</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Nijmegen</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>L.J. Bandell, geregistreerd bedrijfsarts</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-l-j-bandell-geregistreerd-bedrijfsarts-lochem-3024897</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Velhorst</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>7241TB</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Lochem</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Mepros Bedrijfsgezondheidsdienst</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-mepros-bedrijfsgezondheidsdienst-rotterdam-3022513</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Strevelsweg</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-213</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>3083AS</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Rotterdam</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Praktijk voor Orthomanuele Geneeskunde J.M. Kuipers-Krouwel</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-praktijk-voor-orthomanuele-geneeskunde-j-m-kuipers-krouwel-huizen-128670</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Vliegheiweg</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1272PH</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Huizen</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Acupuncture by Kim</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-acupuncture-by-kim-amsterdam-10026862</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Veembroederhof</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>185</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1019HD</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Amsterdam</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Cohesie</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-cohesie-voorthuizen-3045800</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Baron van Nagellstraat</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>3781AP</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Voorthuizen</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NEXT Bedrijfsartsen</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-next-bedrijfsartsen-nijmegen-10018010</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Prins Hendrikstraat</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>6521AW</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Nijmegen</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Acupunctuurpraktijk The</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-acupunctuurpraktijk-the-bussum-179920</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Lindelaan</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1405AJ</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Bussum</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Van Altena en De Jongh Bedrijfsartsen</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-van-altena-en-de-jongh-bedrijfsartsen-alkmaar-3029921</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Robijnstraat</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1812RB</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Alkmaar</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Acupunctuur Werkt, Esther van Dorst</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-acupunctuur-werkt-esther-van-dorst-utrecht-3044017</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Amsterdamsestraatweg</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>699</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>3555HD</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Ale van der Veen, arts Orthomanuele geneeskunde</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-ale-van-der-veen-arts-orthomanuele-geneeskunde-heemstede-224622</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Roemer Visscherplein</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2106AG</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Heemstede</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Arbo- en reïntegratiebedrijf</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Van Zitteren Bedrijfsarts en Luchtvaartgeneeskundige</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/arbo-en-reintegratiebedrijf-van-zitteren-bedrijfsarts-en-luchtvaartgeneeskundige-roosendaal-3038884</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Krekelberg</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>116</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>4708KP</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Roosendaal</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor Acupunctuur A.H. Suhendra</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-artsenpraktijk-voor-acupunctuur-a-h-suhendra-amstelveen-225376</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Turfschip</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>1186XL</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Amstelveen</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor homeopathie Laila Alberts</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-artsenpraktijk-voor-homeopathie-laila-alberts-hilversum-225819</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Eikbosserweg</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>236</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>1213SC</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Hilversum</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Centrum voor Holistische Geneeskunst</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-centrum-voor-holistische-geneeskunst-ellecom-219501</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>de Friedhof</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>6955BP</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Ellecom</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>De Jonge Biotherapie</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-de-jonge-biotherapie-oosterhout-3031012</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Warandelaan</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>4904PD</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Oosterhout</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Homeopatische praktijk Jan Bol</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-homeopatische-praktijk-jan-bol-groningen-225671</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Kometenstraat</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>9742EC</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Groningen</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>In Manu Medici, specialist bewegingsapparaat</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-in-manu-medici-specialist-bewegingsapparaat-houten-3031048</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Tingietersgilde</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>3994XP</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Houten</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Medisch Centrum Acupunctuur</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-medisch-centrum-acupunctuur-bergen-241226</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Prins Hendriklaan</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>1862EL</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Bergen</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Mediwellness, Acupunctuur</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-mediwellness-acupunctuur-haarlem-3034079</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Vlietsorgstraat</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2012JB</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Haarlem</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Miriam Schumacher, arts, Praktijk voor Integrale Geneeskunde</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-miriam-schumacher-arts-praktijk-voor-integrale-geneeskunde-castricum-219218</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Willem de Zwijgerlaan</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>114</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>1901CT</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Castricum</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Artsenpraktijk voor alternatieve geneeskunde</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Newmedix</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/artsenpraktijk-voor-alternatieve-geneeskunde-newmedix-best-3063245</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Bosseweg</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>5682BA</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Best</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
         <is>
           <t>2025-05-27</t>
         </is>

</xml_diff>